<commit_message>
final run on python and androis, save outputs
</commit_message>
<xml_diff>
--- a/python/output/DF_Full_Result.xlsx
+++ b/python/output/DF_Full_Result.xlsx
@@ -450,19 +450,19 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>43.72934953371684</v>
+        <v>57.49022531509399</v>
       </c>
       <c r="C2" t="n">
-        <v>8.488205269934554</v>
+        <v>5.100912131091908</v>
       </c>
       <c r="D2" t="n">
-        <v>3.743371725082397</v>
+        <v>4.491315841674805</v>
       </c>
       <c r="E2" t="n">
-        <v>1.256757361407309</v>
+        <v>0.8420841797982249</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -473,7 +473,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I2" t="n">
         <v>256</v>
@@ -485,23 +485,23 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{'anOptimizer': 'adam', 'batch_size': 10, 'epochs': 8, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+          <t>{'anOptimizer': 'adam', 'batch_size': 10, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.9212598204612732</v>
+        <v>0.913385808467865</v>
       </c>
       <c r="M2" t="n">
         <v>0.9448819160461426</v>
       </c>
       <c r="N2" t="n">
-        <v>0.920634925365448</v>
+        <v>0.9126983880996704</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9289255539576212</v>
+        <v>0.923655370871226</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0112857355924842</v>
+        <v>0.01501205741479679</v>
       </c>
       <c r="Q2" t="n">
         <v>1</v>
@@ -509,19 +509,19 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>55.10249098141988</v>
+        <v>39.78802744547526</v>
       </c>
       <c r="C3" t="n">
-        <v>6.693594823139848</v>
+        <v>1.423466044835468</v>
       </c>
       <c r="D3" t="n">
-        <v>4.923126697540283</v>
+        <v>2.929161310195923</v>
       </c>
       <c r="E3" t="n">
-        <v>2.831712622961212</v>
+        <v>0.03748435253047754</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I3" t="n">
         <v>256</v>
@@ -544,43 +544,43 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{'anOptimizer': 'adam', 'batch_size': 10, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+          <t>{'anOptimizer': 'adam', 'batch_size': 10, 'epochs': 8, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0.9212598204612732</v>
+        <v>0.9291338324546814</v>
       </c>
       <c r="M3" t="n">
         <v>0.9448819160461426</v>
       </c>
       <c r="N3" t="n">
-        <v>0.920634925365448</v>
+        <v>0.89682537317276</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9289255539576212</v>
+        <v>0.923613707224528</v>
       </c>
       <c r="P3" t="n">
-        <v>0.0112857355924842</v>
+        <v>0.02000352744147469</v>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>45.43693908055624</v>
+        <v>57.74329535166422</v>
       </c>
       <c r="C4" t="n">
-        <v>8.522634457513245</v>
+        <v>7.589177844387023</v>
       </c>
       <c r="D4" t="n">
-        <v>4.093569119771321</v>
+        <v>5.998699903488159</v>
       </c>
       <c r="E4" t="n">
-        <v>1.445325663825754</v>
+        <v>3.080780681821662</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -591,7 +591,7 @@
         <v>50</v>
       </c>
       <c r="H4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I4" t="n">
         <v>256</v>
@@ -603,23 +603,23 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{'anOptimizer': 'adam', 'batch_size': 50, 'epochs': 8, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+          <t>{'anOptimizer': 'adam', 'batch_size': 50, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.6535432934761047</v>
+        <v>0.7401574850082397</v>
       </c>
       <c r="M4" t="n">
-        <v>0.834645688533783</v>
+        <v>0.8897637724876404</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8095238208770752</v>
+        <v>0.7222222089767456</v>
       </c>
       <c r="O4" t="n">
-        <v>0.7659042676289877</v>
+        <v>0.7840478221575419</v>
       </c>
       <c r="P4" t="n">
-        <v>0.08011041731293501</v>
+        <v>0.07511020857037724</v>
       </c>
       <c r="Q4" t="n">
         <v>3</v>
@@ -627,19 +627,19 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>63.74553982416789</v>
+        <v>53.27555712064107</v>
       </c>
       <c r="C5" t="n">
-        <v>9.184282472261263</v>
+        <v>11.65337900211236</v>
       </c>
       <c r="D5" t="n">
-        <v>3.67401917775472</v>
+        <v>3.023576895395915</v>
       </c>
       <c r="E5" t="n">
-        <v>1.501417548428905</v>
+        <v>0.2767486985329319</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -650,7 +650,7 @@
         <v>50</v>
       </c>
       <c r="H5" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5" t="n">
         <v>256</v>
@@ -662,23 +662,23 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{'anOptimizer': 'adam', 'batch_size': 50, 'epochs': 10, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
+          <t>{'anOptimizer': 'adam', 'batch_size': 50, 'epochs': 8, 'hidUnit': 256, 'outActivation': 'softmax'}</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0.6771653294563293</v>
+        <v>0.6220472455024719</v>
       </c>
       <c r="M5" t="n">
-        <v>0.6929134130477905</v>
+        <v>0.7637795209884644</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8650793433189392</v>
+        <v>0.761904776096344</v>
       </c>
       <c r="O5" t="n">
-        <v>0.745052695274353</v>
+        <v>0.7159105141957601</v>
       </c>
       <c r="P5" t="n">
-        <v>0.08511481545463608</v>
+        <v>0.06637576653389871</v>
       </c>
       <c r="Q5" t="n">
         <v>4</v>

</xml_diff>